<commit_message>
updates for spring 2016
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emonson/Dropbox/Sites/FridayForum/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>status</t>
   </si>
@@ -97,6 +102,12 @@
   </si>
   <si>
     <t>Fall_2015</t>
+  </si>
+  <si>
+    <t>Spring_2016</t>
+  </si>
+  <si>
+    <t>future</t>
   </si>
 </sst>
 </file>
@@ -196,6 +207,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -521,13 +537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
@@ -535,7 +551,7 @@
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -549,292 +565,299 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="16">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
         <v>42179</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
         <v>41984</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
         <v>41814</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16">
-      <c r="A6" s="4" t="s">
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
         <v>41632</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16">
-      <c r="A7" s="4" t="s">
+      <c r="D7" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
         <v>41449</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16">
-      <c r="A8" s="4" t="s">
+      <c r="D8" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
         <v>41267</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="16">
-      <c r="A9" s="4" t="s">
+      <c r="D9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
         <v>41084</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16">
-      <c r="A10" s="4" t="s">
+      <c r="D10" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
         <v>40901</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
         <v>40718</v>
       </c>
-      <c r="D11" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16">
-      <c r="A12" s="4" t="s">
+      <c r="D12" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
         <v>40536</v>
       </c>
-      <c r="D12" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16">
-      <c r="A13" s="4" t="s">
+      <c r="D13" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
         <v>40353</v>
       </c>
-      <c r="D13" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
         <v>40171</v>
       </c>
-      <c r="D14" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16">
-      <c r="A15" s="4" t="s">
+      <c r="D15" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
         <v>39988</v>
       </c>
-      <c r="D15" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16">
-      <c r="A16" s="4" t="s">
+      <c r="D16" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
         <v>39806</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16">
-      <c r="A17" s="4" t="s">
+      <c r="D17" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
         <v>39623</v>
       </c>
-      <c r="D17" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16">
-      <c r="A18" s="4" t="s">
+      <c r="D18" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5">
         <v>39440</v>
       </c>
-      <c r="D18" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16">
-      <c r="A19" s="4" t="s">
+      <c r="D19" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
         <v>39257</v>
       </c>
-      <c r="D19" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16">
-      <c r="A20" s="4" t="s">
+      <c r="D20" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
         <v>39075</v>
       </c>
-      <c r="D20" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16">
-      <c r="A21" s="4" t="s">
+      <c r="D21" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
         <v>38892</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated cached files and site about a month ago and forgot to push changes
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>status</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Spring_2016</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
 </sst>
 </file>
@@ -540,7 +537,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,11 +567,11 @@
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -582,11 +579,13 @@
         <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>42348</v>
+      </c>
       <c r="D3" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -600,7 +599,7 @@
         <v>42179</v>
       </c>
       <c r="D4" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -614,7 +613,7 @@
         <v>41984</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
shifted back to CS personal site
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>status</t>
   </si>
@@ -105,6 +108,15 @@
   </si>
   <si>
     <t>Spring_2016</t>
+  </si>
+  <si>
+    <t>Fall_2016</t>
+  </si>
+  <si>
+    <t>Spring_2017</t>
+  </si>
+  <si>
+    <t>future</t>
   </si>
 </sst>
 </file>
@@ -534,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,67 +576,63 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1">
-        <v>0.6</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>42545</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
         <v>42348</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
-        <v>42179</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>41984</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>41814</v>
+        <v>42179</v>
       </c>
       <c r="D6" s="1">
         <v>0.05</v>
@@ -632,13 +640,13 @@
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5">
-        <v>41632</v>
+        <v>41984</v>
       </c>
       <c r="D7" s="1">
         <v>0.05</v>
@@ -646,13 +654,13 @@
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>41449</v>
+        <v>41814</v>
       </c>
       <c r="D8" s="1">
         <v>0.05</v>
@@ -660,28 +668,27 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5">
-        <v>41267</v>
+        <v>41632</v>
       </c>
       <c r="D9" s="1">
         <v>0.05</v>
       </c>
-      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
-        <v>41084</v>
+        <v>41449</v>
       </c>
       <c r="D10" s="1">
         <v>0.05</v>
@@ -689,27 +696,28 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5">
-        <v>40901</v>
+        <v>41267</v>
       </c>
       <c r="D11" s="1">
         <v>0.05</v>
       </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>40718</v>
+        <v>41084</v>
       </c>
       <c r="D12" s="1">
         <v>0.05</v>
@@ -717,13 +725,13 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5">
-        <v>40536</v>
+        <v>40901</v>
       </c>
       <c r="D13" s="1">
         <v>0.05</v>
@@ -731,13 +739,13 @@
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>40353</v>
+        <v>40718</v>
       </c>
       <c r="D14" s="1">
         <v>0.05</v>
@@ -745,13 +753,13 @@
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="5">
-        <v>40171</v>
+        <v>40536</v>
       </c>
       <c r="D15" s="1">
         <v>0.05</v>
@@ -759,13 +767,13 @@
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="5">
-        <v>39988</v>
+        <v>40353</v>
       </c>
       <c r="D16" s="1">
         <v>0.05</v>
@@ -773,13 +781,13 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="5">
-        <v>39806</v>
+        <v>40171</v>
       </c>
       <c r="D17" s="1">
         <v>0.05</v>
@@ -787,13 +795,13 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="5">
-        <v>39623</v>
+        <v>39988</v>
       </c>
       <c r="D18" s="1">
         <v>0.05</v>
@@ -801,13 +809,13 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>39440</v>
+        <v>39806</v>
       </c>
       <c r="D19" s="1">
         <v>0.05</v>
@@ -815,13 +823,13 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="5">
-        <v>39257</v>
+        <v>39623</v>
       </c>
       <c r="D20" s="1">
         <v>0.05</v>
@@ -829,13 +837,13 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="5">
-        <v>39075</v>
+        <v>39440</v>
       </c>
       <c r="D21" s="1">
         <v>0.05</v>
@@ -843,15 +851,43 @@
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
+        <v>39257</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5">
+        <v>39075</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
         <v>38892</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D24" s="1">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
spring 2017 made current
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>status</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Spring_2017</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
 </sst>
 </file>
@@ -549,7 +546,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,21 +576,25 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>42714</v>
+      </c>
       <c r="D3" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -607,7 +608,7 @@
         <v>42545</v>
       </c>
       <c r="D4" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -621,7 +622,7 @@
         <v>42348</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
initiated Fall 2017 semester
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>status</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>Spring_2017</t>
+  </si>
+  <si>
+    <t>Fall_2017</t>
+  </si>
+  <si>
+    <t>Spring_2018</t>
+  </si>
+  <si>
+    <t>future</t>
   </si>
 </sst>
 </file>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,83 +580,76 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
-        <v>42714</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>42545</v>
+        <v>42910</v>
       </c>
       <c r="D4" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42714</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42545</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
         <v>42348</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>42179</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
-        <v>41984</v>
       </c>
       <c r="D7" s="1">
         <v>0.05</v>
@@ -655,13 +657,13 @@
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>41814</v>
+        <v>42179</v>
       </c>
       <c r="D8" s="1">
         <v>0.05</v>
@@ -669,13 +671,13 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5">
-        <v>41632</v>
+        <v>41984</v>
       </c>
       <c r="D9" s="1">
         <v>0.05</v>
@@ -683,13 +685,13 @@
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
-        <v>41449</v>
+        <v>41814</v>
       </c>
       <c r="D10" s="1">
         <v>0.05</v>
@@ -697,28 +699,27 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5">
-        <v>41267</v>
+        <v>41632</v>
       </c>
       <c r="D11" s="1">
         <v>0.05</v>
       </c>
-      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>41084</v>
+        <v>41449</v>
       </c>
       <c r="D12" s="1">
         <v>0.05</v>
@@ -726,27 +727,28 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5">
-        <v>40901</v>
+        <v>41267</v>
       </c>
       <c r="D13" s="1">
         <v>0.05</v>
       </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>40718</v>
+        <v>41084</v>
       </c>
       <c r="D14" s="1">
         <v>0.05</v>
@@ -754,13 +756,13 @@
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="5">
-        <v>40536</v>
+        <v>40901</v>
       </c>
       <c r="D15" s="1">
         <v>0.05</v>
@@ -768,13 +770,13 @@
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="5">
-        <v>40353</v>
+        <v>40718</v>
       </c>
       <c r="D16" s="1">
         <v>0.05</v>
@@ -782,13 +784,13 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="5">
-        <v>40171</v>
+        <v>40536</v>
       </c>
       <c r="D17" s="1">
         <v>0.05</v>
@@ -796,13 +798,13 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="5">
-        <v>39988</v>
+        <v>40353</v>
       </c>
       <c r="D18" s="1">
         <v>0.05</v>
@@ -810,13 +812,13 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>39806</v>
+        <v>40171</v>
       </c>
       <c r="D19" s="1">
         <v>0.05</v>
@@ -824,13 +826,13 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="5">
-        <v>39623</v>
+        <v>39988</v>
       </c>
       <c r="D20" s="1">
         <v>0.05</v>
@@ -838,13 +840,13 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="5">
-        <v>39440</v>
+        <v>39806</v>
       </c>
       <c r="D21" s="1">
         <v>0.05</v>
@@ -852,13 +854,13 @@
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="5">
-        <v>39257</v>
+        <v>39623</v>
       </c>
       <c r="D22" s="1">
         <v>0.05</v>
@@ -866,13 +868,13 @@
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="5">
-        <v>39075</v>
+        <v>39440</v>
       </c>
       <c r="D23" s="1">
         <v>0.05</v>
@@ -880,15 +882,43 @@
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
+        <v>39257</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
+        <v>39075</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
         <v>38892</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D26" s="1">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setting spring 2018 to current
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>status</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>Spring_2018</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
 </sst>
 </file>
@@ -555,7 +552,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,7 +582,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -593,10 +593,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>43079</v>
       </c>
       <c r="D3" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -610,7 +613,7 @@
         <v>42910</v>
       </c>
       <c r="D4" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -624,7 +627,7 @@
         <v>42714</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fall 2018 semester added
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emonson/Dropbox/Sites/FridayForum/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7FDF9B-5F48-4948-A171-40DA01F90C89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>status</t>
   </si>
@@ -120,13 +121,16 @@
   </si>
   <si>
     <t>Spring_2018</t>
+  </si>
+  <si>
+    <t>Fall_2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +180,20 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -201,7 +219,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,6 +227,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -222,6 +242,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -548,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,40 +600,41 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="1">
         <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5">
-        <v>43079</v>
+        <v>43275</v>
       </c>
       <c r="D3" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>42910</v>
+        <v>43079</v>
       </c>
       <c r="D4" s="1">
         <v>0.1</v>
@@ -618,13 +642,13 @@
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5">
-        <v>42714</v>
+        <v>42910</v>
       </c>
       <c r="D5" s="1">
         <v>0.05</v>
@@ -632,13 +656,13 @@
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>42545</v>
+        <v>42714</v>
       </c>
       <c r="D6" s="1">
         <v>0.05</v>
@@ -646,27 +670,27 @@
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>42545</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
         <v>42348</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
-        <v>42179</v>
       </c>
       <c r="D8" s="1">
         <v>0.05</v>
@@ -674,13 +698,13 @@
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5">
-        <v>41984</v>
+        <v>42179</v>
       </c>
       <c r="D9" s="1">
         <v>0.05</v>
@@ -688,13 +712,13 @@
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="5">
-        <v>41814</v>
+        <v>41984</v>
       </c>
       <c r="D10" s="1">
         <v>0.05</v>
@@ -702,13 +726,13 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5">
-        <v>41632</v>
+        <v>41814</v>
       </c>
       <c r="D11" s="1">
         <v>0.05</v>
@@ -716,13 +740,13 @@
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>41449</v>
+        <v>41632</v>
       </c>
       <c r="D12" s="1">
         <v>0.05</v>
@@ -730,42 +754,42 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5">
-        <v>41267</v>
+        <v>41449</v>
       </c>
       <c r="D13" s="1">
         <v>0.05</v>
       </c>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>41084</v>
+        <v>41267</v>
       </c>
       <c r="D14" s="1">
         <v>0.05</v>
       </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="5">
-        <v>40901</v>
+        <v>41084</v>
       </c>
       <c r="D15" s="1">
         <v>0.05</v>
@@ -773,13 +797,13 @@
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="5">
-        <v>40718</v>
+        <v>40901</v>
       </c>
       <c r="D16" s="1">
         <v>0.05</v>
@@ -787,13 +811,13 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="5">
-        <v>40536</v>
+        <v>40718</v>
       </c>
       <c r="D17" s="1">
         <v>0.05</v>
@@ -801,13 +825,13 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="5">
-        <v>40353</v>
+        <v>40536</v>
       </c>
       <c r="D18" s="1">
         <v>0.05</v>
@@ -815,13 +839,13 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>40171</v>
+        <v>40353</v>
       </c>
       <c r="D19" s="1">
         <v>0.05</v>
@@ -829,13 +853,13 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="5">
-        <v>39988</v>
+        <v>40171</v>
       </c>
       <c r="D20" s="1">
         <v>0.05</v>
@@ -843,13 +867,13 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="5">
-        <v>39806</v>
+        <v>39988</v>
       </c>
       <c r="D21" s="1">
         <v>0.05</v>
@@ -857,13 +881,13 @@
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="5">
-        <v>39623</v>
+        <v>39806</v>
       </c>
       <c r="D22" s="1">
         <v>0.05</v>
@@ -871,13 +895,13 @@
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="5">
-        <v>39440</v>
+        <v>39623</v>
       </c>
       <c r="D23" s="1">
         <v>0.05</v>
@@ -885,13 +909,13 @@
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="5">
-        <v>39257</v>
+        <v>39440</v>
       </c>
       <c r="D24" s="1">
         <v>0.05</v>
@@ -899,13 +923,13 @@
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="5">
-        <v>39075</v>
+        <v>39257</v>
       </c>
       <c r="D25" s="1">
         <v>0.05</v>
@@ -913,15 +937,29 @@
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
+        <v>39075</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5">
         <v>38892</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D27" s="1">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating to spring 2019 current
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emonson/Dropbox/Sites/FridayForum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7FDF9B-5F48-4948-A171-40DA01F90C89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3EF6E2-9F13-7E4B-8AE9-E002B90E7E52}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>status</t>
   </si>
@@ -124,13 +124,16 @@
   </si>
   <si>
     <t>Fall_2018</t>
+  </si>
+  <si>
+    <t>Spring_2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,7 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -572,13 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
@@ -586,7 +590,7 @@
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -600,9 +604,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="17">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -612,354 +616,368 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
-        <v>43275</v>
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="17">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>43444</v>
       </c>
       <c r="D3" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="17">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>43079</v>
+        <v>43275</v>
       </c>
       <c r="D4" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="17">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>43079</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="6" customFormat="1" ht="17">
+      <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
         <v>42910</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="6" customFormat="1" ht="17">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
         <v>42714</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="D7" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="17">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
         <v>42545</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="D8" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="17">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
         <v>42348</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="D9" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17">
+      <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
         <v>42179</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="D10" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
         <v>41984</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
         <v>41814</v>
       </c>
-      <c r="D11" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="D12" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
         <v>41632</v>
       </c>
-      <c r="D12" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="D13" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
         <v>41449</v>
       </c>
-      <c r="D13" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
         <v>41267</v>
       </c>
-      <c r="D14" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="D15" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="17">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
         <v>41084</v>
       </c>
-      <c r="D15" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="D16" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
         <v>40901</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="D17" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17">
+      <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
         <v>40718</v>
       </c>
-      <c r="D17" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="D18" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5">
         <v>40536</v>
       </c>
-      <c r="D18" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="D19" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17">
+      <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
         <v>40353</v>
       </c>
-      <c r="D19" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="D20" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17">
+      <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
         <v>40171</v>
       </c>
-      <c r="D20" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="D21" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17">
+      <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
         <v>39988</v>
       </c>
-      <c r="D21" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="D22" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17">
+      <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5">
         <v>39806</v>
       </c>
-      <c r="D22" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="D23" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17">
+      <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
         <v>39623</v>
       </c>
-      <c r="D23" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="D24" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17">
+      <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
         <v>39440</v>
       </c>
-      <c r="D24" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="D25" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17">
+      <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
         <v>39257</v>
       </c>
-      <c r="D25" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="D26" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17">
+      <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5">
         <v>39075</v>
       </c>
-      <c r="D26" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="D27" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17">
+      <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5">
         <v>38892</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fall 2019 initial mods
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emonson/Dropbox/Sites/FridayForum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3EF6E2-9F13-7E4B-8AE9-E002B90E7E52}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4BCF2F-7AC5-8448-BF2E-94E667192F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>status</t>
   </si>
@@ -127,13 +127,22 @@
   </si>
   <si>
     <t>Spring_2019</t>
+  </si>
+  <si>
+    <t>Spring_2020</t>
+  </si>
+  <si>
+    <t>Fall_2019</t>
+  </si>
+  <si>
+    <t>future</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -576,13 +585,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
@@ -590,7 +599,7 @@
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -604,380 +613,404 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="17">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="17">
-      <c r="A3" s="7" t="s">
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>43640</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
         <v>43444</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="17">
-      <c r="A4" s="1" t="s">
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
         <v>43275</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="17">
-      <c r="A5" s="1" t="s">
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
         <v>43079</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="17">
-      <c r="A6" s="4" t="s">
+      <c r="D7" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
         <v>42910</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="17">
-      <c r="A7" s="4" t="s">
+      <c r="D8" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
         <v>42714</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="17">
-      <c r="A8" s="4" t="s">
+      <c r="D9" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
         <v>42545</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" ht="17">
-      <c r="A9" s="4" t="s">
+      <c r="D10" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
         <v>42348</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17">
-      <c r="A10" s="4" t="s">
+      <c r="D11" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
         <v>42179</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="4" t="s">
+      <c r="D12" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
         <v>41984</v>
       </c>
-      <c r="D11" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="4" t="s">
+      <c r="D13" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
         <v>41814</v>
       </c>
-      <c r="D12" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17">
-      <c r="A13" s="4" t="s">
+      <c r="D14" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
         <v>41632</v>
       </c>
-      <c r="D13" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="4" t="s">
+      <c r="D15" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
         <v>41449</v>
       </c>
-      <c r="D14" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17">
-      <c r="A15" s="4" t="s">
+      <c r="D16" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
         <v>41267</v>
       </c>
-      <c r="D15" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="17">
-      <c r="A16" s="4" t="s">
+      <c r="D17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
         <v>41084</v>
       </c>
-      <c r="D16" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17">
-      <c r="A17" s="4" t="s">
+      <c r="D18" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5">
         <v>40901</v>
       </c>
-      <c r="D17" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17">
-      <c r="A18" s="4" t="s">
+      <c r="D19" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
         <v>40718</v>
       </c>
-      <c r="D18" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17">
-      <c r="A19" s="4" t="s">
+      <c r="D20" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
         <v>40536</v>
       </c>
-      <c r="D19" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17">
-      <c r="A20" s="4" t="s">
+      <c r="D21" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
         <v>40353</v>
       </c>
-      <c r="D20" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17">
-      <c r="A21" s="4" t="s">
+      <c r="D22" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5">
         <v>40171</v>
       </c>
-      <c r="D21" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17">
-      <c r="A22" s="4" t="s">
+      <c r="D23" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
         <v>39988</v>
       </c>
-      <c r="D22" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17">
-      <c r="A23" s="4" t="s">
+      <c r="D24" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
         <v>39806</v>
       </c>
-      <c r="D23" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17">
-      <c r="A24" s="4" t="s">
+      <c r="D25" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
         <v>39623</v>
       </c>
-      <c r="D24" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17">
-      <c r="A25" s="4" t="s">
+      <c r="D26" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5">
         <v>39440</v>
       </c>
-      <c r="D25" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17">
-      <c r="A26" s="4" t="s">
+      <c r="D27" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5">
         <v>39257</v>
       </c>
-      <c r="D26" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17">
-      <c r="A27" s="4" t="s">
+      <c r="D28" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5">
         <v>39075</v>
       </c>
-      <c r="D27" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17">
-      <c r="A28" s="4" t="s">
+      <c r="D29" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
         <v>38892</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D30" s="1">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prep for spring 2020
</commit_message>
<xml_diff>
--- a/SheetNames.xlsx
+++ b/SheetNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emonson/Dropbox/Sites/FridayForum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4BCF2F-7AC5-8448-BF2E-94E667192F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF197A-2E94-4C41-B83D-1D6019C180D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>status</t>
   </si>
@@ -133,16 +133,13 @@
   </si>
   <si>
     <t>Fall_2019</t>
-  </si>
-  <si>
-    <t>future</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -588,10 +585,10 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
@@ -599,7 +596,7 @@
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -613,29 +610,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>43444</v>
+      </c>
       <c r="D3" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -646,10 +647,10 @@
         <v>43640</v>
       </c>
       <c r="D4" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -660,10 +661,10 @@
         <v>43444</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="17">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -677,7 +678,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="17">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -691,7 +692,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -705,7 +706,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -719,7 +720,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -733,7 +734,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="6" customFormat="1" ht="17">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -747,7 +748,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -761,7 +762,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -775,7 +776,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -789,7 +790,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -803,7 +804,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -817,7 +818,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -832,7 +833,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -846,7 +847,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
@@ -860,7 +861,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -874,7 +875,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17">
       <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
@@ -888,7 +889,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -902,7 +903,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
@@ -916,7 +917,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="17">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -930,7 +931,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -944,7 +945,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="17">
       <c r="A26" s="4" t="s">
         <v>17</v>
       </c>
@@ -958,7 +959,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="17">
       <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
@@ -972,7 +973,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="17">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -986,7 +987,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="17">
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>

</xml_diff>